<commit_message>
small fix function name and run table
</commit_message>
<xml_diff>
--- a/scripts/stability_testing/Stability_test_setup.xlsx
+++ b/scripts/stability_testing/Stability_test_setup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivergjorvad/Desktop/masteroppgave/OpenEMPIRE/scripts/remaining_runs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivergjorvad/Desktop/forked-OpenEMPIRE/OpenEMPIRE/scripts/stability_testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C6B839-6025-B64C-8357-E998871B77C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE94C30A-B63D-AB48-BB6E-2A068EB91333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{C6EF8596-1DEB-486E-9320-EAC364E6D036}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{C6EF8596-1DEB-486E-9320-EAC364E6D036}"/>
   </bookViews>
   <sheets>
     <sheet name="OOS" sheetId="2" r:id="rId1"/>
@@ -241,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -264,15 +264,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1908DA29-993A-4254-934B-ADACC207CD3E}">
   <dimension ref="B2:O39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A20" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="L38" sqref="D14:L38"/>
     </sheetView>
   </sheetViews>
@@ -655,7 +650,7 @@
       </c>
       <c r="L6" s="10">
         <f ca="1">HOUR(NOW())+MAX(I15:I22)*24-IF(MAX(I15:I22)&gt;1,48,24)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
@@ -757,7 +752,7 @@
       <c r="D15" s="13">
         <v>1</v>
       </c>
-      <c r="E15" s="28" t="str">
+      <c r="E15" t="str">
         <f>"6-"&amp;B15</f>
         <v>6-1</v>
       </c>
@@ -1003,7 +998,6 @@
         <f>B21</f>
         <v>4</v>
       </c>
-      <c r="C22" s="20"/>
       <c r="D22" s="13">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -1224,33 +1218,33 @@
         <v>7</v>
       </c>
       <c r="C28" s="18"/>
-      <c r="D28" s="27">
+      <c r="D28" s="13">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="E28" s="27" t="str">
+      <c r="E28" s="13" t="str">
         <f t="shared" si="1"/>
         <v>6-7</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="20">
-        <v>100</v>
-      </c>
-      <c r="H28" s="20">
-        <v>5</v>
-      </c>
-      <c r="I28" s="21">
+      <c r="G28">
+        <v>100</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28" s="5">
         <f t="shared" si="2"/>
         <v>2.0833333333333335</v>
       </c>
-      <c r="J28" s="21"/>
-      <c r="K28" s="20">
+      <c r="J28" s="5"/>
+      <c r="K28">
         <f>L27+1</f>
         <v>6</v>
       </c>
-      <c r="L28" s="20">
+      <c r="L28">
         <f>K28+H28-1</f>
         <v>10</v>
       </c>
@@ -1261,33 +1255,33 @@
         <v>8</v>
       </c>
       <c r="C29" s="18"/>
-      <c r="D29" s="27">
+      <c r="D29" s="13">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="E29" s="27" t="str">
+      <c r="E29" s="13" t="str">
         <f t="shared" si="1"/>
         <v>6-8</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="20">
-        <v>100</v>
-      </c>
-      <c r="H29" s="20">
-        <v>5</v>
-      </c>
-      <c r="I29" s="21">
+      <c r="G29">
+        <v>100</v>
+      </c>
+      <c r="H29">
+        <v>5</v>
+      </c>
+      <c r="I29" s="5">
         <f t="shared" si="2"/>
         <v>2.0833333333333335</v>
       </c>
-      <c r="J29" s="21"/>
-      <c r="K29" s="20">
+      <c r="J29" s="5"/>
+      <c r="K29">
         <f t="shared" ref="K29:K32" si="8">L28+1</f>
         <v>11</v>
       </c>
-      <c r="L29" s="20">
+      <c r="L29">
         <f t="shared" ref="L29:L32" si="9">K29+H29-1</f>
         <v>15</v>
       </c>
@@ -1297,33 +1291,33 @@
         <f>B29</f>
         <v>8</v>
       </c>
-      <c r="D30" s="27">
+      <c r="D30" s="13">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="E30" s="27" t="str">
+      <c r="E30" s="13" t="str">
         <f t="shared" si="1"/>
         <v>6-8</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="F30" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="20">
-        <v>100</v>
-      </c>
-      <c r="H30" s="20">
-        <v>5</v>
-      </c>
-      <c r="I30" s="21">
+      <c r="G30">
+        <v>100</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+      <c r="I30" s="5">
         <f t="shared" si="2"/>
         <v>2.0833333333333335</v>
       </c>
-      <c r="J30" s="21"/>
-      <c r="K30" s="20">
+      <c r="J30" s="5"/>
+      <c r="K30">
         <f t="shared" si="8"/>
         <v>16</v>
       </c>
-      <c r="L30" s="20">
+      <c r="L30">
         <f t="shared" si="9"/>
         <v>20</v>
       </c>
@@ -1333,33 +1327,33 @@
         <f>B29+1</f>
         <v>9</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D31" s="13">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="E31" s="27" t="str">
+      <c r="E31" s="13" t="str">
         <f t="shared" si="1"/>
         <v>6-9</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="20">
-        <v>100</v>
-      </c>
-      <c r="H31" s="20">
-        <v>5</v>
-      </c>
-      <c r="I31" s="21">
+      <c r="G31">
+        <v>100</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31" s="5">
         <f t="shared" si="2"/>
         <v>2.0833333333333335</v>
       </c>
-      <c r="J31" s="21"/>
-      <c r="K31" s="20">
+      <c r="J31" s="5"/>
+      <c r="K31">
         <f t="shared" si="8"/>
         <v>21</v>
       </c>
-      <c r="L31" s="20">
+      <c r="L31">
         <f t="shared" si="9"/>
         <v>25</v>
       </c>
@@ -1427,10 +1421,10 @@
         <v>2.0833333333333335</v>
       </c>
       <c r="J33" s="5"/>
-      <c r="K33" s="20">
+      <c r="K33">
         <v>1</v>
       </c>
-      <c r="L33" s="20">
+      <c r="L33">
         <f>K33+H33-1</f>
         <v>5</v>
       </c>
@@ -1544,7 +1538,7 @@
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B37" s="20">
+      <c r="B37">
         <f>B35+1</f>
         <v>12</v>
       </c>
@@ -1580,54 +1574,46 @@
       </c>
     </row>
     <row r="38" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="24">
+      <c r="B38" s="21">
         <f>B37</f>
         <v>12</v>
       </c>
-      <c r="D38" s="25">
+      <c r="D38" s="22">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="E38" s="25" t="str">
+      <c r="E38" s="22" t="str">
         <f t="shared" si="1"/>
         <v>6-12</v>
       </c>
-      <c r="F38" s="24" t="s">
+      <c r="F38" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G38" s="24">
-        <v>100</v>
-      </c>
-      <c r="H38" s="24">
-        <v>5</v>
-      </c>
-      <c r="I38" s="26">
+      <c r="G38" s="21">
+        <v>100</v>
+      </c>
+      <c r="H38" s="21">
+        <v>5</v>
+      </c>
+      <c r="I38" s="23">
         <f t="shared" si="2"/>
         <v>2.0833333333333335</v>
       </c>
-      <c r="J38" s="26"/>
-      <c r="K38" s="24">
+      <c r="J38" s="23"/>
+      <c r="K38" s="21">
         <f t="shared" si="10"/>
         <v>26</v>
       </c>
-      <c r="L38" s="24">
+      <c r="L38" s="21">
         <f t="shared" si="11"/>
         <v>30</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="D39" s="20"/>
-      <c r="E39" s="20">
+      <c r="E39">
         <f>COUNTA(_xlfn.UNIQUE(E15:E38))</f>
         <v>12</v>
       </c>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1640,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7920B913-4F2C-4CFA-8D08-F22EED9E69BF}">
-  <dimension ref="C3:N45"/>
+  <dimension ref="C3:M45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1659,61 +1645,52 @@
     <col min="13" max="13" width="26.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="N3" s="20"/>
-    </row>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="M3" s="20"/>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C4" s="3">
         <v>10</v>
       </c>
       <c r="D4" s="17">
         <v>0.3</v>
       </c>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-    </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C5" s="3">
         <v>50</v>
       </c>
       <c r="D5" s="15">
         <v>2</v>
       </c>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-    </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C6" s="3">
         <v>100</v>
       </c>
       <c r="D6" s="15">
         <v>4</v>
       </c>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-    </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-    </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
         <v>1</v>
       </c>
@@ -1733,7 +1710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" s="11" t="s">
         <v>15</v>
       </c>
@@ -1756,44 +1733,44 @@
       </c>
       <c r="K12" s="10">
         <f ca="1">HOUR(NOW())+MAX(H21:H44)*24-IF(MAX(H21:H44)&gt;1,48,24)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C13" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="20">
-        <v>100</v>
-      </c>
-      <c r="E13" s="20">
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
         <v>10</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="5">
         <f t="shared" ref="F13:F15" si="0">_xlfn.XLOOKUP(D13,$C$4:$C$6,$D$4:$D$6)*E13/24</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="H13" s="8"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C14" s="22" t="s">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="20">
-        <v>100</v>
-      </c>
-      <c r="E14" s="20">
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14">
         <v>10</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="5">
         <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="H14" s="8"/>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" s="6" t="s">
         <v>18</v>
       </c>
@@ -1844,7 +1821,7 @@
       <c r="C21" s="13">
         <v>1</v>
       </c>
-      <c r="D21" s="28" t="str">
+      <c r="D21" t="str">
         <f>"6-"&amp;C21</f>
         <v>6-1</v>
       </c>
@@ -2253,129 +2230,129 @@
       </c>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C34" s="27">
+      <c r="C34" s="13">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="D34" s="27" t="str">
+      <c r="D34" s="13" t="str">
         <f t="shared" si="1"/>
         <v>6-14</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="20">
-        <v>100</v>
-      </c>
-      <c r="G34" s="20">
-        <v>5</v>
-      </c>
-      <c r="H34" s="21">
+      <c r="F34">
+        <v>100</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+      <c r="H34" s="5">
         <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="20">
+      <c r="I34" s="5"/>
+      <c r="J34">
         <f>K33+1</f>
         <v>6</v>
       </c>
-      <c r="K34" s="20">
+      <c r="K34">
         <f>J34+G34-1</f>
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C35" s="27">
+      <c r="C35" s="13">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="D35" s="27" t="str">
+      <c r="D35" s="13" t="str">
         <f t="shared" si="1"/>
         <v>6-15</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="20">
-        <v>100</v>
-      </c>
-      <c r="G35" s="20">
-        <v>5</v>
-      </c>
-      <c r="H35" s="21">
+      <c r="F35">
+        <v>100</v>
+      </c>
+      <c r="G35">
+        <v>5</v>
+      </c>
+      <c r="H35" s="5">
         <f t="shared" ref="H35:H38" si="10">_xlfn.XLOOKUP(F35,$C$4:$C$6,$D$4:$D$6)*G35/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="I35" s="21"/>
-      <c r="J35" s="20">
+      <c r="I35" s="5"/>
+      <c r="J35">
         <f t="shared" ref="J35:J38" si="11">K34+1</f>
         <v>11</v>
       </c>
-      <c r="K35" s="20">
+      <c r="K35">
         <f t="shared" ref="K35:K38" si="12">J35+G35-1</f>
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C36" s="27">
+      <c r="C36" s="13">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="D36" s="27" t="str">
+      <c r="D36" s="13" t="str">
         <f t="shared" si="1"/>
         <v>6-16</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="E36" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="20">
-        <v>100</v>
-      </c>
-      <c r="G36" s="20">
-        <v>5</v>
-      </c>
-      <c r="H36" s="21">
+      <c r="F36">
+        <v>100</v>
+      </c>
+      <c r="G36">
+        <v>5</v>
+      </c>
+      <c r="H36" s="5">
         <f t="shared" si="10"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="I36" s="21"/>
-      <c r="J36" s="20">
+      <c r="I36" s="5"/>
+      <c r="J36">
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="K36" s="20">
+      <c r="K36">
         <f t="shared" si="12"/>
         <v>20</v>
       </c>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C37" s="27">
+      <c r="C37" s="13">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="D37" s="27" t="str">
+      <c r="D37" s="13" t="str">
         <f t="shared" si="1"/>
         <v>6-17</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="E37" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="20">
-        <v>100</v>
-      </c>
-      <c r="G37" s="20">
-        <v>5</v>
-      </c>
-      <c r="H37" s="21">
+      <c r="F37">
+        <v>100</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="H37" s="5">
         <f t="shared" si="10"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="I37" s="21"/>
-      <c r="J37" s="20">
+      <c r="I37" s="5"/>
+      <c r="J37">
         <f t="shared" si="11"/>
         <v>21</v>
       </c>
-      <c r="K37" s="20">
+      <c r="K37">
         <f t="shared" si="12"/>
         <v>25</v>
       </c>
@@ -2435,10 +2412,10 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="I39" s="5"/>
-      <c r="J39" s="20">
+      <c r="J39">
         <v>1</v>
       </c>
-      <c r="K39" s="20">
+      <c r="K39">
         <f>J39+G39-1</f>
         <v>5</v>
       </c>
@@ -2572,50 +2549,42 @@
       </c>
     </row>
     <row r="44" spans="3:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="25">
+      <c r="C44" s="22">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="D44" s="25" t="str">
+      <c r="D44" s="22" t="str">
         <f t="shared" si="1"/>
         <v>6-24</v>
       </c>
-      <c r="E44" s="24" t="s">
+      <c r="E44" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="24">
-        <v>100</v>
-      </c>
-      <c r="G44" s="24">
-        <v>5</v>
-      </c>
-      <c r="H44" s="26">
+      <c r="F44" s="21">
+        <v>100</v>
+      </c>
+      <c r="G44" s="21">
+        <v>5</v>
+      </c>
+      <c r="H44" s="23">
         <f t="shared" ref="H44" si="16">_xlfn.XLOOKUP(F44,$C$4:$C$6,$D$4:$D$6)*G44/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="I44" s="26"/>
-      <c r="J44" s="24">
+      <c r="I44" s="23"/>
+      <c r="J44" s="21">
         <f t="shared" si="14"/>
         <v>26</v>
       </c>
-      <c r="K44" s="24">
+      <c r="K44" s="21">
         <f t="shared" si="15"/>
         <v>30</v>
       </c>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C45" s="20"/>
-      <c r="D45" s="20">
+      <c r="D45">
         <f>COUNTA(_xlfn.UNIQUE(D21:D44))</f>
         <v>24</v>
       </c>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>